<commit_message>
Day 2 end of day
</commit_message>
<xml_diff>
--- a/Day 2 - Lab 1 - Employee Summary.xlsx
+++ b/Day 2 - Lab 1 - Employee Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kroger_Training\Excel_Class_Files\Student_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AF6E50AF-655C-4D2B-87DC-30AD167F7422}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{578061D9-3391-427F-BDEB-C22E568A2F83}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -237,7 +237,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>